<commit_message>
Add cleaned and error data files
</commit_message>
<xml_diff>
--- a/validate_data/errors.xlsx
+++ b/validate_data/errors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,69 +518,1021 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Matilda</t>
+          <t>Peter</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Johansson</t>
+          <t>Englund</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1967-12-30</t>
+          <t>1959-05-13</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+46 70-222 39 66</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>+46 72-848 57 32</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>peter.englundicloud.com</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Dalkarlsberg</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>71392</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Gyttorp</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Nora</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2024-11-19</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>USB Hub</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>3061</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>299</v>
+      </c>
+      <c r="P2" t="n">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kjell</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jönsson</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1971-09-24</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>kjell.jonsson@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Private</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Brånan</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>84552</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Åsarna</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Berg</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2024-11-24</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Adjustable Lamp</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>3064</v>
-      </c>
-      <c r="N2" t="n">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Bullerbacken Fågelsjövägen 19</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>82770</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Los</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Ljusdal</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2024-10-08</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Webcam</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>3009</v>
+      </c>
+      <c r="N3" t="n">
         <v>4</v>
       </c>
-      <c r="O2" t="n">
-        <v>14824.77</v>
-      </c>
-      <c r="P2" t="n">
-        <v>59299.08</v>
+      <c r="O3" t="n">
+        <v>699</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2796</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Emil</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Eklund</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2003-06-02</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>emil.eklund@icloud.com</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Himmer 850</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>71595</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Kilsmo</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Örebro</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2024-08-12</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Desk</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>3005</v>
+      </c>
+      <c r="N4" t="n">
+        <v>4</v>
+      </c>
+      <c r="O4" t="n">
+        <v>5550</v>
+      </c>
+      <c r="P4" t="n">
+        <v>22200</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Roland</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Isaksson</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1994-04-01</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>+46 70-331 20 22</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Folkströmsvägen</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>61273</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Hjortkvarn</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Hallsberg</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2024-08-05</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Whiteboard</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>3022</v>
+      </c>
+      <c r="N5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O5" t="n">
+        <v>899</v>
+      </c>
+      <c r="P5" t="n">
+        <v>3596</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ingegärd</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Danielsson</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1994-12-28</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>+46 70-358 26 64</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ingegard.danielssonlive.com</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Pryssgårdsvägen 1</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>61176</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nävekvarn</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nyköping</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2024-07-16</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Soundbar</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>3036</v>
+      </c>
+      <c r="N6" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2600</v>
+      </c>
+      <c r="P6" t="n">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Rut</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jönsson</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1989-02-16</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>+46 70-980 99 83</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>rut.jonssonhotmail.com</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Hemvägen</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>77010</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Fredriksberg</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Ludvika</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2024-07-03</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Wireless Mouse</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>3068</v>
+      </c>
+      <c r="N7" t="n">
+        <v>3</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1200</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Lena</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Pettersson</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1961-05-28</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>+46 73-238 97 15</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>lena.petterssonoutlook.com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Flokanvägen 61</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>78199</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Idkerberget</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Borlänge</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Gaming Mouse</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>3016</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1300</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Josefine</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Hansen</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1994-03-19</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>+46 72-877 20 76</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>josefine.hansenlive.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Björnhyttan Ljungåsen Olsjön</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>77290</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Grängesberg</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Ludvika</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Microphone</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>3010</v>
+      </c>
+      <c r="N9" t="n">
+        <v>4</v>
+      </c>
+      <c r="O9" t="n">
+        <v>999</v>
+      </c>
+      <c r="P9" t="n">
+        <v>3996</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Olof</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sjöberg</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2001-04-24</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>+46 70-526 28 17</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>olof.sjobergicloud.com</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Olatjärn Kronstugan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>82776</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Ramsjö</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Ljusdal</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2024-05-11</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Speaker System</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>3048</v>
+      </c>
+      <c r="N10" t="n">
+        <v>3</v>
+      </c>
+      <c r="O10" t="n">
+        <v>13500</v>
+      </c>
+      <c r="P10" t="n">
+        <v>40500</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Arne</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Holmqvist</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2003-09-07</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>+46 76-640 10 54</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>arne.holmqvisthotmail.com</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Björkbergsvägen</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>82771</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Hamra</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Ljusdal</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>2024-04-29</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Webcam</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>3009</v>
+      </c>
+      <c r="N11" t="n">
+        <v>5</v>
+      </c>
+      <c r="O11" t="n">
+        <v>699</v>
+      </c>
+      <c r="P11" t="n">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Anders</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Eriksson</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1993-02-28</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>+46 76-625 56 64</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Hillersbergsvägen</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>84398</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Sörbygden</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Bräcke</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>2024-04-10</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>USB Flash Drive</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>3015</v>
+      </c>
+      <c r="N12" t="n">
+        <v>5</v>
+      </c>
+      <c r="O12" t="n">
+        <v>799</v>
+      </c>
+      <c r="P12" t="n">
+        <v>3995</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mari</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Persson</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2000-04-17</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>+46 70-221 12 37</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>mari.perssonhotmail.com</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Rönneshytta Station Fixan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>69497</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Rönneshytta</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Askersund</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2024-02-03</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>3001</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
+        <v>8999</v>
+      </c>
+      <c r="P13" t="n">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Joakim</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Olsson</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1988-04-20</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>+46 72-422 50 70</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>joakim.olssonlive.com</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Storhullsjön 203</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>86496</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Stöde</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Sundsvall</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>2024-01-31</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Thunderbolt Cable</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>3062</v>
+      </c>
+      <c r="N14" t="n">
+        <v>4</v>
+      </c>
+      <c r="O14" t="n">
+        <v>499</v>
+      </c>
+      <c r="P14" t="n">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Birgitta</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Bergström</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1954-04-19</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>+46 72-956 54 42</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>birgitta.bergstromhotmail.com</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Gårdsjövägen</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>82772</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Korskrogen</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Ljusdal</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>2024-01-24</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>HDMI Cable</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>3046</v>
+      </c>
+      <c r="N15" t="n">
+        <v>2</v>
+      </c>
+      <c r="O15" t="n">
+        <v>100</v>
+      </c>
+      <c r="P15" t="n">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>